<commit_message>
Modificato id worksheet per la colonna -id
</commit_message>
<xml_diff>
--- a/Dataset_xlsx/symptoms2.xlsx
+++ b/Dataset_xlsx/symptoms2.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="chief_complaint_id" sheetId="1" r:id="rId1"/>
+    <sheet name="_id" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="999999"/>
 </workbook>
@@ -1551,11 +1551,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I390"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>